<commit_message>
CH updates selections and adds categories
</commit_message>
<xml_diff>
--- a/Data/urls and tweet names.xlsx
+++ b/Data/urls and tweet names.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colej\Documents\Research projects\covid_leaders_gender\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01329C74-B479-4E2E-AE8A-4F2122BBB2F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B894DAD-AF46-4AAE-A3E4-0E141372631A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{914505A7-F87C-4C92-B14A-1371F970280E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{914505A7-F87C-4C92-B14A-1371F970280E}"/>
   </bookViews>
   <sheets>
     <sheet name="immigration" sheetId="1" r:id="rId1"/>
     <sheet name="covid" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">covid!$A$1:$I$28</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">immigration!$A$1:$I$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">covid!$A$1:$J$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">immigration!$A$1:$J$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="132">
   <si>
     <t>Tweet name</t>
   </si>
@@ -423,6 +423,18 @@
   </si>
   <si>
     <t>maybe</t>
+  </si>
+  <si>
+    <t>selection_category</t>
+  </si>
+  <si>
+    <t>high_trust</t>
+  </si>
+  <si>
+    <t>high_anger</t>
+  </si>
+  <si>
+    <t>control</t>
   </si>
 </sst>
 </file>
@@ -800,20 +812,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B4486E-E01C-4D25-85C4-44DBEAA8987E}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="8" max="9" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -839,10 +851,13 @@
         <v>126</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -868,10 +883,13 @@
         <v>125</v>
       </c>
       <c r="I2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -897,10 +915,13 @@
         <v>125</v>
       </c>
       <c r="I3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -926,10 +947,13 @@
         <v>125</v>
       </c>
       <c r="I4" t="s">
+        <v>129</v>
+      </c>
+      <c r="J4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -948,230 +972,248 @@
       <c r="F5">
         <v>-3.8010000000000002</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>1.427</v>
+      </c>
+      <c r="C6">
+        <v>5.3949999999999996</v>
+      </c>
+      <c r="D6">
+        <v>2.4470000000000001</v>
+      </c>
+      <c r="E6">
+        <v>1.7689999999999999</v>
+      </c>
+      <c r="F6">
+        <v>-3.6259999999999994</v>
+      </c>
+      <c r="H6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>2.3330000000000002</v>
+      </c>
+      <c r="C7">
+        <v>5.4939999999999998</v>
+      </c>
+      <c r="D7">
+        <v>4.7949999999999999</v>
+      </c>
+      <c r="E7">
+        <v>2.012</v>
+      </c>
+      <c r="F7">
+        <v>-3.4819999999999998</v>
+      </c>
+      <c r="H7" t="s">
+        <v>125</v>
+      </c>
+      <c r="I7" t="s">
+        <v>129</v>
+      </c>
+      <c r="J7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>2.105</v>
+      </c>
+      <c r="C8">
+        <v>5.125</v>
+      </c>
+      <c r="D8">
+        <v>2.16</v>
+      </c>
+      <c r="E8">
+        <v>1.7010000000000001</v>
+      </c>
+      <c r="F8">
+        <v>-3.4239999999999999</v>
+      </c>
+      <c r="J8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B6">
+      <c r="B9">
         <v>1.8720000000000001</v>
       </c>
-      <c r="C6">
+      <c r="C9">
         <v>4.9160000000000004</v>
       </c>
-      <c r="D6">
+      <c r="D9">
         <v>2.0760000000000001</v>
       </c>
-      <c r="E6">
+      <c r="E9">
         <v>1.597</v>
       </c>
-      <c r="F6">
+      <c r="F9">
         <v>-3.3190000000000004</v>
       </c>
-      <c r="G6" t="s">
-        <v>125</v>
-      </c>
-      <c r="H6" t="s">
-        <v>125</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="G9" t="s">
+        <v>125</v>
+      </c>
+      <c r="H9" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7">
-        <v>2.105</v>
-      </c>
-      <c r="C7">
-        <v>5.125</v>
-      </c>
-      <c r="D7">
-        <v>2.16</v>
-      </c>
-      <c r="E7">
-        <v>1.7010000000000001</v>
-      </c>
-      <c r="F7">
-        <v>-3.4239999999999999</v>
-      </c>
-      <c r="I7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8">
-        <v>1.427</v>
-      </c>
-      <c r="C8">
-        <v>5.3949999999999996</v>
-      </c>
-      <c r="D8">
-        <v>2.4470000000000001</v>
-      </c>
-      <c r="E8">
-        <v>1.7689999999999999</v>
-      </c>
-      <c r="F8">
-        <v>-3.6259999999999994</v>
-      </c>
-      <c r="I8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>1.56</v>
+      </c>
+      <c r="C10">
+        <v>5.25</v>
+      </c>
+      <c r="D10">
+        <v>2.2890000000000001</v>
+      </c>
+      <c r="E10">
+        <v>1.9610000000000001</v>
+      </c>
+      <c r="F10">
+        <v>-3.2889999999999997</v>
+      </c>
+      <c r="G10" t="s">
+        <v>125</v>
+      </c>
+      <c r="J10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>1.2370000000000001</v>
+      </c>
+      <c r="C11">
+        <v>5.2649999999999997</v>
+      </c>
+      <c r="D11">
+        <v>3.7970000000000002</v>
+      </c>
+      <c r="E11">
+        <v>2.359</v>
+      </c>
+      <c r="F11">
+        <v>-2.9059999999999997</v>
+      </c>
+      <c r="J11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>29</v>
       </c>
-      <c r="B9">
+      <c r="B12">
         <v>1.8480000000000001</v>
       </c>
-      <c r="C9">
+      <c r="C12">
         <v>4.6379999999999999</v>
       </c>
-      <c r="D9">
+      <c r="D12">
         <v>1.77</v>
       </c>
-      <c r="E9">
+      <c r="E12">
         <v>1.899</v>
       </c>
-      <c r="F9">
+      <c r="F12">
         <v>-2.7389999999999999</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>1.8380000000000001</v>
+      </c>
+      <c r="C13">
+        <v>5.2590000000000003</v>
+      </c>
+      <c r="D13">
+        <v>3.4359999999999999</v>
+      </c>
+      <c r="E13">
+        <v>2.8479999999999999</v>
+      </c>
+      <c r="F13">
+        <v>-2.4110000000000005</v>
+      </c>
+      <c r="G13" t="s">
+        <v>125</v>
+      </c>
+      <c r="J13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="B10">
+      <c r="B14">
         <v>1.85</v>
       </c>
-      <c r="C10">
+      <c r="C14">
         <v>4.3410000000000002</v>
       </c>
-      <c r="D10">
+      <c r="D14">
         <v>1.57</v>
       </c>
-      <c r="E10">
+      <c r="E14">
         <v>1.95</v>
       </c>
-      <c r="F10">
+      <c r="F14">
         <v>-2.391</v>
       </c>
-      <c r="I10" t="s">
+      <c r="H14" t="s">
+        <v>125</v>
+      </c>
+      <c r="I14" t="s">
+        <v>131</v>
+      </c>
+      <c r="J14" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11">
-        <v>1.56</v>
-      </c>
-      <c r="C11">
-        <v>5.25</v>
-      </c>
-      <c r="D11">
-        <v>2.2890000000000001</v>
-      </c>
-      <c r="E11">
-        <v>1.9610000000000001</v>
-      </c>
-      <c r="F11">
-        <v>-3.2889999999999997</v>
-      </c>
-      <c r="G11" t="s">
-        <v>125</v>
-      </c>
-      <c r="H11" t="s">
-        <v>125</v>
-      </c>
-      <c r="I11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12">
-        <v>2.3330000000000002</v>
-      </c>
-      <c r="C12">
-        <v>5.4939999999999998</v>
-      </c>
-      <c r="D12">
-        <v>4.7949999999999999</v>
-      </c>
-      <c r="E12">
-        <v>2.012</v>
-      </c>
-      <c r="F12">
-        <v>-3.4819999999999998</v>
-      </c>
-      <c r="I12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>1.2370000000000001</v>
-      </c>
-      <c r="C13">
-        <v>5.2649999999999997</v>
-      </c>
-      <c r="D13">
-        <v>3.7970000000000002</v>
-      </c>
-      <c r="E13">
-        <v>2.359</v>
-      </c>
-      <c r="F13">
-        <v>-2.9059999999999997</v>
-      </c>
-      <c r="I13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14">
-        <v>2.3769999999999998</v>
-      </c>
-      <c r="C14">
-        <v>4.2590000000000003</v>
-      </c>
-      <c r="D14">
-        <v>1.72</v>
-      </c>
-      <c r="E14">
-        <v>2.3639999999999999</v>
-      </c>
-      <c r="F14">
-        <v>-1.8950000000000005</v>
-      </c>
-      <c r="I14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -1190,144 +1232,156 @@
       <c r="F15">
         <v>-1.9340000000000006</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B16">
-        <v>1.8380000000000001</v>
+        <v>2.3769999999999998</v>
       </c>
       <c r="C16">
-        <v>5.2590000000000003</v>
+        <v>4.2590000000000003</v>
       </c>
       <c r="D16">
-        <v>3.4359999999999999</v>
+        <v>1.72</v>
       </c>
       <c r="E16">
-        <v>2.8479999999999999</v>
+        <v>2.3639999999999999</v>
       </c>
       <c r="F16">
-        <v>-2.4110000000000005</v>
-      </c>
-      <c r="G16" t="s">
-        <v>125</v>
+        <v>-1.8950000000000005</v>
       </c>
       <c r="H16" t="s">
         <v>125</v>
       </c>
       <c r="I16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="J16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>2.4740000000000002</v>
+      </c>
+      <c r="C17">
+        <v>4.415</v>
+      </c>
+      <c r="D17">
+        <v>2.3849999999999998</v>
+      </c>
+      <c r="E17">
+        <v>3.6949999999999998</v>
+      </c>
+      <c r="F17">
+        <v>-0.7200000000000002</v>
+      </c>
+      <c r="H17" t="s">
+        <v>125</v>
+      </c>
+      <c r="I17" t="s">
+        <v>131</v>
+      </c>
+      <c r="J17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>3.7949999999999999</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>3.1829999999999998</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>1.5</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>3.476</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>0.29300000000000015</v>
       </c>
-      <c r="G17" t="s">
-        <v>125</v>
-      </c>
-      <c r="H17" t="s">
-        <v>125</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="G18" t="s">
+        <v>125</v>
+      </c>
+      <c r="H18" t="s">
+        <v>125</v>
+      </c>
+      <c r="I18" t="s">
+        <v>131</v>
+      </c>
+      <c r="J18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>2.4740000000000002</v>
-      </c>
-      <c r="C18">
-        <v>4.415</v>
-      </c>
-      <c r="D18">
-        <v>2.3849999999999998</v>
-      </c>
-      <c r="E18">
-        <v>3.6949999999999998</v>
-      </c>
-      <c r="F18">
-        <v>-0.7200000000000002</v>
-      </c>
-      <c r="I18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>2.8519999999999999</v>
+      </c>
+      <c r="C19">
+        <v>2.9039999999999999</v>
+      </c>
+      <c r="D19">
+        <v>1.6080000000000001</v>
+      </c>
+      <c r="E19">
+        <v>3.9279999999999999</v>
+      </c>
+      <c r="F19">
+        <v>1.024</v>
+      </c>
+      <c r="G19" t="s">
+        <v>125</v>
+      </c>
+      <c r="H19" t="s">
+        <v>127</v>
+      </c>
+      <c r="I19" t="s">
+        <v>131</v>
+      </c>
+      <c r="J19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>26</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>2.7949999999999999</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>2.6349999999999998</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>1.2250000000000001</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>3.698</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <v>1.0630000000000002</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J20" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20">
-        <v>2.8519999999999999</v>
-      </c>
-      <c r="C20">
-        <v>2.9039999999999999</v>
-      </c>
-      <c r="D20">
-        <v>1.6080000000000001</v>
-      </c>
-      <c r="E20">
-        <v>3.9279999999999999</v>
-      </c>
-      <c r="F20">
-        <v>1.024</v>
-      </c>
-      <c r="G20" t="s">
-        <v>125</v>
-      </c>
-      <c r="H20" t="s">
-        <v>127</v>
-      </c>
-      <c r="I20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1346,11 +1400,11 @@
       <c r="F21">
         <v>2.1540000000000004</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1369,207 +1423,219 @@
       <c r="F22">
         <v>2.8380000000000001</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <v>3.548</v>
+      </c>
+      <c r="C23">
+        <v>2.3250000000000002</v>
+      </c>
+      <c r="D23">
+        <v>1.165</v>
+      </c>
+      <c r="E23">
+        <v>6.1150000000000002</v>
+      </c>
+      <c r="F23">
+        <v>3.79</v>
+      </c>
+      <c r="J23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <v>3.58</v>
+      </c>
+      <c r="C24">
+        <v>1.7529999999999999</v>
+      </c>
+      <c r="D24">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="E24">
+        <v>6.2140000000000004</v>
+      </c>
+      <c r="F24">
+        <v>4.4610000000000003</v>
+      </c>
+      <c r="J24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>8</v>
       </c>
-      <c r="B23">
+      <c r="B25">
         <v>4.0979999999999999</v>
       </c>
-      <c r="C23">
+      <c r="C25">
         <v>1.5429999999999999</v>
       </c>
-      <c r="D23">
+      <c r="D25">
         <v>0.73199999999999998</v>
       </c>
-      <c r="E23">
+      <c r="E25">
         <v>6.1070000000000002</v>
       </c>
-      <c r="F23">
+      <c r="F25">
         <v>4.5640000000000001</v>
       </c>
-      <c r="G23" t="s">
-        <v>125</v>
-      </c>
-      <c r="H23" t="s">
-        <v>125</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="G25" t="s">
+        <v>125</v>
+      </c>
+      <c r="H25" t="s">
+        <v>125</v>
+      </c>
+      <c r="I25" t="s">
+        <v>130</v>
+      </c>
+      <c r="J25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24">
-        <v>3.548</v>
-      </c>
-      <c r="C24">
-        <v>2.3250000000000002</v>
-      </c>
-      <c r="D24">
-        <v>1.165</v>
-      </c>
-      <c r="E24">
-        <v>6.1150000000000002</v>
-      </c>
-      <c r="F24">
-        <v>3.79</v>
-      </c>
-      <c r="I24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25">
-        <v>3.58</v>
-      </c>
-      <c r="C25">
-        <v>1.7529999999999999</v>
-      </c>
-      <c r="D25">
-        <v>1.0249999999999999</v>
-      </c>
-      <c r="E25">
-        <v>6.2140000000000004</v>
-      </c>
-      <c r="F25">
-        <v>4.4610000000000003</v>
-      </c>
-      <c r="I25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>3.8919999999999999</v>
+      </c>
+      <c r="C26">
+        <v>2.0859999999999999</v>
+      </c>
+      <c r="D26">
+        <v>1.163</v>
+      </c>
+      <c r="E26">
+        <v>6.7759999999999998</v>
+      </c>
+      <c r="F26">
+        <v>4.6899999999999995</v>
+      </c>
+      <c r="J26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>2</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <v>3.403</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>1.234</v>
       </c>
-      <c r="D26">
+      <c r="D27">
         <v>0.96799999999999997</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <v>6.2210000000000001</v>
       </c>
-      <c r="F26">
+      <c r="F27">
         <v>4.9870000000000001</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J27" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>12</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>5.2149999999999999</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>1.5129999999999999</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <v>1.079</v>
       </c>
-      <c r="E27">
+      <c r="E28">
         <v>6.6790000000000003</v>
       </c>
-      <c r="F27">
+      <c r="F28">
         <v>5.1660000000000004</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>4.516</v>
+      </c>
+      <c r="C29">
+        <v>1.81</v>
+      </c>
+      <c r="D29">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="E29">
         <v>7</v>
       </c>
-      <c r="B28">
+      <c r="F29">
+        <v>5.1899999999999995</v>
+      </c>
+      <c r="H29" t="s">
+        <v>125</v>
+      </c>
+      <c r="I29" t="s">
+        <v>130</v>
+      </c>
+      <c r="J29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30">
         <v>4.0979999999999999</v>
       </c>
-      <c r="C28">
+      <c r="C30">
         <v>1.38</v>
       </c>
-      <c r="D28">
+      <c r="D30">
         <v>0.97399999999999998</v>
       </c>
-      <c r="E28">
+      <c r="E30">
         <v>6.75</v>
       </c>
-      <c r="F28">
+      <c r="F30">
         <v>5.37</v>
       </c>
-      <c r="G28" t="s">
-        <v>125</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="G30" t="s">
+        <v>125</v>
+      </c>
+      <c r="H30" t="s">
         <v>127</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I30" t="s">
+        <v>130</v>
+      </c>
+      <c r="J30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29">
-        <v>3.8919999999999999</v>
-      </c>
-      <c r="C29">
-        <v>2.0859999999999999</v>
-      </c>
-      <c r="D29">
-        <v>1.163</v>
-      </c>
-      <c r="E29">
-        <v>6.7759999999999998</v>
-      </c>
-      <c r="F29">
-        <v>4.6899999999999995</v>
-      </c>
-      <c r="I29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30">
-        <v>4.516</v>
-      </c>
-      <c r="C30">
-        <v>1.81</v>
-      </c>
-      <c r="D30">
-        <v>0.91900000000000004</v>
-      </c>
-      <c r="E30">
-        <v>7</v>
-      </c>
-      <c r="F30">
-        <v>5.1899999999999995</v>
-      </c>
-      <c r="I30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1595,10 +1661,13 @@
         <v>125</v>
       </c>
       <c r="I31" t="s">
+        <v>130</v>
+      </c>
+      <c r="J31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1624,13 +1693,16 @@
         <v>125</v>
       </c>
       <c r="I32" t="s">
+        <v>130</v>
+      </c>
+      <c r="J32" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I32" xr:uid="{F3A6193A-CC72-4EA3-9756-EF782EA4EFA3}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I32">
-      <sortCondition ref="E1:E32"/>
+  <autoFilter ref="A1:J32" xr:uid="{F3A6193A-CC72-4EA3-9756-EF782EA4EFA3}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J32">
+      <sortCondition ref="F1:F32"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1641,20 +1713,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2EED990-D6F7-4EFC-9974-FCEDBCC8E7AD}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1680,27 +1752,30 @@
         <v>126</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B2">
-        <v>6.3860000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="C2">
-        <v>0.86199999999999999</v>
+        <v>6.6269999999999998</v>
       </c>
       <c r="D2">
-        <v>0.70299999999999996</v>
+        <v>2.1230000000000002</v>
       </c>
       <c r="E2">
-        <v>6.4139999999999997</v>
+        <v>0.54</v>
       </c>
       <c r="F2">
-        <v>5.5519999999999996</v>
+        <v>-6.0869999999999997</v>
       </c>
       <c r="G2" t="s">
         <v>125</v>
@@ -1709,50 +1784,62 @@
         <v>125</v>
       </c>
       <c r="I2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="J2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>71</v>
       </c>
       <c r="B3">
-        <v>4.5</v>
+        <v>2.1749999999999998</v>
       </c>
       <c r="C3">
-        <v>1.224</v>
+        <v>6.8029999999999999</v>
       </c>
       <c r="D3">
-        <v>0.80400000000000005</v>
+        <v>3.161</v>
       </c>
       <c r="E3">
-        <v>7.3179999999999996</v>
+        <v>0.91700000000000004</v>
       </c>
       <c r="F3">
-        <v>6.0939999999999994</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-5.8860000000000001</v>
+      </c>
+      <c r="G3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>70</v>
       </c>
       <c r="B4">
-        <v>5.3529999999999998</v>
+        <v>1.8460000000000001</v>
       </c>
       <c r="C4">
-        <v>1.2949999999999999</v>
+        <v>6.5670000000000002</v>
       </c>
       <c r="D4">
-        <v>0.98399999999999999</v>
+        <v>2.8</v>
       </c>
       <c r="E4">
-        <v>7.6379999999999999</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="F4">
-        <v>6.343</v>
+        <v>-5.71</v>
       </c>
       <c r="G4" t="s">
         <v>125</v>
@@ -1761,284 +1848,311 @@
         <v>125</v>
       </c>
       <c r="I4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="J4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="B5">
-        <v>4.2</v>
+        <v>1.167</v>
       </c>
       <c r="C5">
-        <v>1.403</v>
+        <v>6.4790000000000001</v>
       </c>
       <c r="D5">
-        <v>1.0980000000000001</v>
+        <v>5.5350000000000001</v>
       </c>
       <c r="E5">
-        <v>7.1029999999999998</v>
+        <v>0.877</v>
       </c>
       <c r="F5">
-        <v>5.6999999999999993</v>
+        <v>-5.6020000000000003</v>
+      </c>
+      <c r="H5" t="s">
+        <v>125</v>
       </c>
       <c r="I5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="J5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="B6">
-        <v>2.0310000000000001</v>
+        <v>1.2190000000000001</v>
       </c>
       <c r="C6">
-        <v>1.5</v>
+        <v>6.2859999999999996</v>
       </c>
       <c r="D6">
-        <v>0.83099999999999996</v>
+        <v>5.8550000000000004</v>
       </c>
       <c r="E6">
-        <v>8.1489999999999991</v>
+        <v>0.86899999999999999</v>
       </c>
       <c r="F6">
-        <v>6.6489999999999991</v>
-      </c>
-      <c r="G6" t="s">
-        <v>125</v>
-      </c>
-      <c r="H6" t="s">
-        <v>125</v>
-      </c>
-      <c r="I6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-5.4169999999999998</v>
+      </c>
+      <c r="J6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B7">
-        <v>2.4529999999999998</v>
+        <v>1.1859999999999999</v>
       </c>
       <c r="C7">
-        <v>1.5229999999999999</v>
+        <v>6.1369999999999996</v>
       </c>
       <c r="D7">
-        <v>0.80600000000000005</v>
+        <v>1.806</v>
       </c>
       <c r="E7">
-        <v>7.5739999999999998</v>
+        <v>0.84799999999999998</v>
       </c>
       <c r="F7">
-        <v>6.0510000000000002</v>
-      </c>
-      <c r="I7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-5.2889999999999997</v>
+      </c>
+      <c r="G7" t="s">
+        <v>125</v>
+      </c>
+      <c r="J7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B8">
-        <v>4.75</v>
+        <v>1.71</v>
       </c>
       <c r="C8">
-        <v>1.6</v>
+        <v>6.1879999999999997</v>
       </c>
       <c r="D8">
-        <v>1.25</v>
+        <v>3.891</v>
       </c>
       <c r="E8">
-        <v>8.4290000000000003</v>
+        <v>0.95</v>
       </c>
       <c r="F8">
-        <v>6.8290000000000006</v>
-      </c>
-      <c r="G8" t="s">
-        <v>125</v>
+        <v>-5.2379999999999995</v>
       </c>
       <c r="H8" t="s">
         <v>125</v>
       </c>
       <c r="I8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="J8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B9">
-        <v>4.9560000000000004</v>
+        <v>1.079</v>
       </c>
       <c r="C9">
-        <v>1.6719999999999999</v>
+        <v>5.6870000000000003</v>
       </c>
       <c r="D9">
-        <v>1.127</v>
+        <v>3.1539999999999999</v>
       </c>
       <c r="E9">
-        <v>6.8239999999999998</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="F9">
-        <v>5.1520000000000001</v>
-      </c>
-      <c r="H9" t="s">
-        <v>125</v>
-      </c>
-      <c r="I9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-5.0540000000000003</v>
+      </c>
+      <c r="G9" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="B10">
-        <v>5.2990000000000004</v>
+        <v>1.4750000000000001</v>
       </c>
       <c r="C10">
-        <v>1.8460000000000001</v>
+        <v>5.8479999999999999</v>
       </c>
       <c r="D10">
-        <v>0.82799999999999996</v>
+        <v>5.2389999999999999</v>
       </c>
       <c r="E10">
-        <v>6.2839999999999998</v>
+        <v>0.95099999999999996</v>
       </c>
       <c r="F10">
-        <v>4.4379999999999997</v>
-      </c>
-      <c r="I10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-4.8970000000000002</v>
+      </c>
+      <c r="G10" t="s">
+        <v>125</v>
+      </c>
+      <c r="J10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B11">
-        <v>3.532</v>
+        <v>1.4710000000000001</v>
       </c>
       <c r="C11">
-        <v>2.6669999999999998</v>
+        <v>5.8819999999999997</v>
       </c>
       <c r="D11">
-        <v>1.2809999999999999</v>
+        <v>2.8180000000000001</v>
       </c>
       <c r="E11">
-        <v>5.758</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>3.0910000000000002</v>
-      </c>
-      <c r="I11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-4.8819999999999997</v>
+      </c>
+      <c r="J11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B12">
-        <v>3.8149999999999999</v>
+        <v>2.29</v>
       </c>
       <c r="C12">
-        <v>3.1059999999999999</v>
+        <v>5.8810000000000002</v>
       </c>
       <c r="D12">
-        <v>1.41</v>
+        <v>2.9060000000000001</v>
       </c>
       <c r="E12">
-        <v>5.4029999999999996</v>
+        <v>1.167</v>
       </c>
       <c r="F12">
-        <v>2.2969999999999997</v>
+        <v>-4.7140000000000004</v>
+      </c>
+      <c r="G12" t="s">
+        <v>125</v>
+      </c>
+      <c r="H12" t="s">
+        <v>125</v>
       </c>
       <c r="I12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="J12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B13">
-        <v>4.319</v>
+        <v>2.569</v>
       </c>
       <c r="C13">
-        <v>4.056</v>
+        <v>5.9420000000000002</v>
       </c>
       <c r="D13">
-        <v>1.536</v>
+        <v>3.806</v>
       </c>
       <c r="E13">
-        <v>1.4430000000000001</v>
+        <v>1.2769999999999999</v>
       </c>
       <c r="F13">
-        <v>-2.613</v>
-      </c>
-      <c r="I13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-4.665</v>
+      </c>
+      <c r="J13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14">
+        <v>1.143</v>
+      </c>
+      <c r="C14">
+        <v>5.0750000000000002</v>
+      </c>
+      <c r="D14">
+        <v>2.831</v>
+      </c>
+      <c r="E14">
+        <v>0.59</v>
+      </c>
+      <c r="F14">
+        <v>-4.4850000000000003</v>
+      </c>
+      <c r="G14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H14" t="s">
+        <v>125</v>
+      </c>
+      <c r="I14" t="s">
+        <v>131</v>
+      </c>
+      <c r="J14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>80</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>2.609</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>5.0289999999999999</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>0.91900000000000004</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>0.67700000000000005</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>-4.3520000000000003</v>
       </c>
-      <c r="I14" t="s">
+      <c r="H15" t="s">
+        <v>125</v>
+      </c>
+      <c r="I15" t="s">
+        <v>131</v>
+      </c>
+      <c r="J15" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15">
-        <v>1.143</v>
-      </c>
-      <c r="C15">
-        <v>5.0750000000000002</v>
-      </c>
-      <c r="D15">
-        <v>2.831</v>
-      </c>
-      <c r="E15">
-        <v>0.59</v>
-      </c>
-      <c r="F15">
-        <v>-4.4850000000000003</v>
-      </c>
-      <c r="G15" t="s">
-        <v>125</v>
-      </c>
-      <c r="H15" t="s">
-        <v>125</v>
-      </c>
-      <c r="I15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -2057,259 +2171,256 @@
       <c r="F16">
         <v>-3.6840000000000002</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B17">
-        <v>1.079</v>
+        <v>4.319</v>
       </c>
       <c r="C17">
-        <v>5.6870000000000003</v>
+        <v>4.056</v>
       </c>
       <c r="D17">
-        <v>3.1539999999999999</v>
+        <v>1.536</v>
       </c>
       <c r="E17">
-        <v>0.63300000000000001</v>
+        <v>1.4430000000000001</v>
       </c>
       <c r="F17">
-        <v>-5.0540000000000003</v>
-      </c>
-      <c r="G17" t="s">
-        <v>125</v>
+        <v>-2.613</v>
       </c>
       <c r="H17" t="s">
         <v>125</v>
       </c>
       <c r="I17" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="J17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B18">
-        <v>1.4750000000000001</v>
+        <v>3.8149999999999999</v>
       </c>
       <c r="C18">
-        <v>5.8479999999999999</v>
+        <v>3.1059999999999999</v>
       </c>
       <c r="D18">
-        <v>5.2389999999999999</v>
+        <v>1.41</v>
       </c>
       <c r="E18">
-        <v>0.95099999999999996</v>
+        <v>5.4029999999999996</v>
       </c>
       <c r="F18">
-        <v>-4.8970000000000002</v>
-      </c>
-      <c r="G18" t="s">
-        <v>125</v>
-      </c>
-      <c r="H18" t="s">
-        <v>125</v>
-      </c>
-      <c r="I18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2.2969999999999997</v>
+      </c>
+      <c r="J18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B19">
-        <v>2.29</v>
+        <v>3.532</v>
       </c>
       <c r="C19">
-        <v>5.8810000000000002</v>
+        <v>2.6669999999999998</v>
       </c>
       <c r="D19">
-        <v>2.9060000000000001</v>
+        <v>1.2809999999999999</v>
       </c>
       <c r="E19">
-        <v>1.167</v>
+        <v>5.758</v>
       </c>
       <c r="F19">
-        <v>-4.7140000000000004</v>
-      </c>
-      <c r="G19" t="s">
-        <v>125</v>
-      </c>
-      <c r="H19" t="s">
-        <v>125</v>
-      </c>
-      <c r="I19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3.0910000000000002</v>
+      </c>
+      <c r="J19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="B20">
-        <v>1.4710000000000001</v>
+        <v>5.2990000000000004</v>
       </c>
       <c r="C20">
-        <v>5.8819999999999997</v>
+        <v>1.8460000000000001</v>
       </c>
       <c r="D20">
-        <v>2.8180000000000001</v>
+        <v>0.82799999999999996</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>6.2839999999999998</v>
       </c>
       <c r="F20">
-        <v>-4.8819999999999997</v>
-      </c>
-      <c r="I20" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4.4379999999999997</v>
+      </c>
+      <c r="J20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B21">
-        <v>2.569</v>
+        <v>4.9560000000000004</v>
       </c>
       <c r="C21">
-        <v>5.9420000000000002</v>
+        <v>1.6719999999999999</v>
       </c>
       <c r="D21">
-        <v>3.806</v>
+        <v>1.127</v>
       </c>
       <c r="E21">
-        <v>1.2769999999999999</v>
+        <v>6.8239999999999998</v>
       </c>
       <c r="F21">
-        <v>-4.665</v>
-      </c>
-      <c r="I21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5.1520000000000001</v>
+      </c>
+      <c r="J21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B22">
-        <v>1.1859999999999999</v>
+        <v>6.3860000000000001</v>
       </c>
       <c r="C22">
-        <v>6.1369999999999996</v>
+        <v>0.86199999999999999</v>
       </c>
       <c r="D22">
-        <v>1.806</v>
+        <v>0.70299999999999996</v>
       </c>
       <c r="E22">
-        <v>0.84799999999999998</v>
+        <v>6.4139999999999997</v>
       </c>
       <c r="F22">
-        <v>-5.2889999999999997</v>
+        <v>5.5519999999999996</v>
       </c>
       <c r="G22" t="s">
         <v>125</v>
       </c>
-      <c r="H22" t="s">
-        <v>125</v>
-      </c>
-      <c r="I22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="B23">
-        <v>1.71</v>
+        <v>4.2</v>
       </c>
       <c r="C23">
-        <v>6.1879999999999997</v>
+        <v>1.403</v>
       </c>
       <c r="D23">
-        <v>3.891</v>
+        <v>1.0980000000000001</v>
       </c>
       <c r="E23">
-        <v>0.95</v>
+        <v>7.1029999999999998</v>
       </c>
       <c r="F23">
-        <v>-5.2379999999999995</v>
-      </c>
-      <c r="I23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5.6999999999999993</v>
+      </c>
+      <c r="J23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B24">
-        <v>1.2190000000000001</v>
+        <v>2.4529999999999998</v>
       </c>
       <c r="C24">
-        <v>6.2859999999999996</v>
+        <v>1.5229999999999999</v>
       </c>
       <c r="D24">
-        <v>5.8550000000000004</v>
+        <v>0.80600000000000005</v>
       </c>
       <c r="E24">
-        <v>0.86899999999999999</v>
+        <v>7.5739999999999998</v>
       </c>
       <c r="F24">
-        <v>-5.4169999999999998</v>
+        <v>6.0510000000000002</v>
+      </c>
+      <c r="H24" t="s">
+        <v>125</v>
       </c>
       <c r="I24" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="J24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="B25">
-        <v>1.167</v>
+        <v>4.5</v>
       </c>
       <c r="C25">
-        <v>6.4790000000000001</v>
+        <v>1.224</v>
       </c>
       <c r="D25">
-        <v>5.5350000000000001</v>
+        <v>0.80400000000000005</v>
       </c>
       <c r="E25">
-        <v>0.877</v>
+        <v>7.3179999999999996</v>
       </c>
       <c r="F25">
-        <v>-5.6020000000000003</v>
+        <v>6.0939999999999994</v>
+      </c>
+      <c r="H25" t="s">
+        <v>125</v>
       </c>
       <c r="I25" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="B26">
-        <v>1.8460000000000001</v>
+        <v>5.3529999999999998</v>
       </c>
       <c r="C26">
-        <v>6.5670000000000002</v>
+        <v>1.2949999999999999</v>
       </c>
       <c r="D26">
-        <v>2.8</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="E26">
-        <v>0.85699999999999998</v>
+        <v>7.6379999999999999</v>
       </c>
       <c r="F26">
-        <v>-5.71</v>
+        <v>6.343</v>
       </c>
       <c r="G26" t="s">
         <v>125</v>
@@ -2318,56 +2429,62 @@
         <v>125</v>
       </c>
       <c r="I26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="J26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="B27">
+        <v>2.0310000000000001</v>
+      </c>
+      <c r="C27">
+        <v>1.5</v>
+      </c>
+      <c r="D27">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="E27">
+        <v>8.1489999999999991</v>
+      </c>
+      <c r="F27">
+        <v>6.6489999999999991</v>
+      </c>
+      <c r="G27" t="s">
+        <v>125</v>
+      </c>
+      <c r="H27" t="s">
+        <v>125</v>
+      </c>
+      <c r="I27" t="s">
+        <v>130</v>
+      </c>
+      <c r="J27" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28">
+        <v>4.75</v>
+      </c>
+      <c r="C28">
         <v>1.6</v>
       </c>
-      <c r="C27">
-        <v>6.6269999999999998</v>
-      </c>
-      <c r="D27">
-        <v>2.1230000000000002</v>
-      </c>
-      <c r="E27">
-        <v>0.54</v>
-      </c>
-      <c r="F27">
-        <v>-6.0869999999999997</v>
-      </c>
-      <c r="G27" t="s">
-        <v>125</v>
-      </c>
-      <c r="H27" t="s">
-        <v>125</v>
-      </c>
-      <c r="I27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28">
-        <v>2.1749999999999998</v>
-      </c>
-      <c r="C28">
-        <v>6.8029999999999999</v>
-      </c>
       <c r="D28">
-        <v>3.161</v>
+        <v>1.25</v>
       </c>
       <c r="E28">
-        <v>0.91700000000000004</v>
+        <v>8.4290000000000003</v>
       </c>
       <c r="F28">
-        <v>-5.8860000000000001</v>
+        <v>6.8290000000000006</v>
       </c>
       <c r="G28" t="s">
         <v>125</v>
@@ -2376,18 +2493,21 @@
         <v>125</v>
       </c>
       <c r="I28" t="s">
-        <v>93</v>
+        <v>130</v>
+      </c>
+      <c r="J28" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I28" xr:uid="{126BD3DF-1197-4B07-A469-03E2E8EA072E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I28">
-      <sortCondition ref="C1:C28"/>
+  <autoFilter ref="A1:J28" xr:uid="{126BD3DF-1197-4B07-A469-03E2E8EA072E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J28">
+      <sortCondition ref="F1:F28"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1" xr:uid="{E6CFD2E4-EC6E-40E2-A316-72E26ADF8E2A}"/>
+    <hyperlink ref="J25" r:id="rId1" xr:uid="{E6CFD2E4-EC6E-40E2-A316-72E26ADF8E2A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>